<commit_message>
Update combined DA results of meta (MetaboDiff) and prot.xlsx
</commit_message>
<xml_diff>
--- a/Pathway analysis/combined DA results of meta (MetaboDiff) and prot.xlsx
+++ b/Pathway analysis/combined DA results of meta (MetaboDiff) and prot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/34420f5773a88cdb/Documents/UM documents/BMS Year 3/Internship ^M Thesis/Sabrina_BMS_Bachelor-Internship/Pathway analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{3BC8C0FD-7778-4C36-A9DE-BC964B352173}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0D89CC7B-9D7F-4D1C-8B06-CD07587EC2E6}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{3BC8C0FD-7778-4C36-A9DE-BC964B352173}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6C5F22D9-64BD-49C2-A9A2-BB923B2AD509}"/>
   <bookViews>
-    <workbookView xWindow="9630" yWindow="0" windowWidth="9730" windowHeight="9740" xr2:uid="{E6E67FF1-58FE-44AC-8594-96B7730F6308}"/>
+    <workbookView xWindow="9340" yWindow="0" windowWidth="9890" windowHeight="10150" xr2:uid="{E6E67FF1-58FE-44AC-8594-96B7730F6308}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2222,8 +2222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F1EEFB-1095-4827-9539-7C4D1444A304}">
   <dimension ref="A1:E626"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>